<commit_message>
🐡💴 Updated with Glitch
</commit_message>
<xml_diff>
--- a/filesxls/personal_budget2.xlsx
+++ b/filesxls/personal_budget2.xlsx
@@ -3024,22 +3024,22 @@
     <row customHeight="1" ht="30" r="5" s="47">
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 31/10/2022</t>
+          <t xml:space="preserve"> 02/11/2022</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>21:37:03</t>
+          <t>19:23:23</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Arriendo </t>
+          <t xml:space="preserve">Juan Camilo </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>800</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">

</xml_diff>

<commit_message>
🔭🍛 Updated with Glitch
</commit_message>
<xml_diff>
--- a/filesxls/personal_budget2.xlsx
+++ b/filesxls/personal_budget2.xlsx
@@ -3024,22 +3024,22 @@
     <row customHeight="1" ht="30" r="5" s="47">
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 02/11/2022</t>
+          <t xml:space="preserve"> 09/11/2022</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>19:23:23</t>
+          <t>19:11:15</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Juan Camilo </t>
+          <t xml:space="preserve">almuerzo </t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>5000</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">

</xml_diff>